<commit_message>
task 7 - Adding Allure setup and report to existing tests
</commit_message>
<xml_diff>
--- a/task3/src/test/resources/testData.xlsx
+++ b/task3/src/test/resources/testData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kzlot\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kzlot\IdeaProjects\fast-track-atqc-java\task3\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728EDB45-3067-49DC-B195-34D980286E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F829C3A-69A2-4B1B-B659-35F3087E711B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{B5B7B252-5BE0-4B7E-AC58-FA2F7C7B5918}"/>
+    <workbookView xWindow="21840" yWindow="3990" windowWidth="27120" windowHeight="13875" xr2:uid="{B5B7B252-5BE0-4B7E-AC58-FA2F7C7B5918}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,23 +47,29 @@
     <t>Top categories</t>
   </si>
   <si>
-    <t>dropdownTest</t>
-  </si>
-  <si>
-    <t>dropdownTestModified</t>
-  </si>
-  <si>
     <t>EN</t>
+  </si>
+  <si>
+    <t>languageChangeTest</t>
+  </si>
+  <si>
+    <t>languageChangeTestWithFirstHeader</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -89,8 +95,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43FD3F89-B16E-44AF-8299-80D36072D19E}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,20 +457,23 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
+      <c r="A3" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>